<commit_message>
added new files and edited code
</commit_message>
<xml_diff>
--- a/new_file.xlsx
+++ b/new_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Female</t>
   </si>
@@ -25,25 +25,13 @@
     <t>Age_Range</t>
   </si>
   <si>
-    <t>(18, 19]</t>
-  </si>
-  <si>
-    <t>(19, 20]</t>
-  </si>
-  <si>
-    <t>(20, 21]</t>
-  </si>
-  <si>
-    <t>(21, 22]</t>
-  </si>
-  <si>
-    <t>(22, 23]</t>
-  </si>
-  <si>
-    <t>(23, 24]</t>
-  </si>
-  <si>
-    <t>(24, 25]</t>
+    <t>12-15 years</t>
+  </si>
+  <si>
+    <t>15-20 years</t>
+  </si>
+  <si>
+    <t>20-30 years</t>
   </si>
 </sst>
 </file>
@@ -401,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,10 +411,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -434,10 +422,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -445,54 +433,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added file and new codes
</commit_message>
<xml_diff>
--- a/new_file.xlsx
+++ b/new_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Female</t>
   </si>
@@ -25,13 +25,43 @@
     <t>Age_Range</t>
   </si>
   <si>
-    <t>12-15 years</t>
+    <t>10-15 years</t>
   </si>
   <si>
     <t>15-20 years</t>
   </si>
   <si>
-    <t>20-30 years</t>
+    <t>20-25 years</t>
+  </si>
+  <si>
+    <t>25-30 years</t>
+  </si>
+  <si>
+    <t>30-35 years</t>
+  </si>
+  <si>
+    <t>35-40 years</t>
+  </si>
+  <si>
+    <t>40-45 years</t>
+  </si>
+  <si>
+    <t>45-50 years</t>
+  </si>
+  <si>
+    <t>50-55 years</t>
+  </si>
+  <si>
+    <t>55-60 years</t>
+  </si>
+  <si>
+    <t>60-65 years</t>
+  </si>
+  <si>
+    <t>70-75 years</t>
+  </si>
+  <si>
+    <t>75-80 years</t>
   </si>
 </sst>
 </file>
@@ -389,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,10 +452,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -433,10 +463,120 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>